<commit_message>
switch orientation changed. completed
</commit_message>
<xml_diff>
--- a/Docs/Components.xlsx
+++ b/Docs/Components.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cris\Documents\Projects\DodOverdrive\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE28263-7BDA-4402-89C4-2FFCDF44241C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A670531-EA26-474E-9A3F-363E78961AD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
   <si>
     <t>Original DOD 250 Size</t>
   </si>
@@ -43,13 +43,97 @@
   </si>
   <si>
     <t>TL081H</t>
+  </si>
+  <si>
+    <t>Jack</t>
+  </si>
+  <si>
+    <t>NMJ4HCD2</t>
+  </si>
+  <si>
+    <t>FootSwitch</t>
+  </si>
+  <si>
+    <t>Toggle</t>
+  </si>
+  <si>
+    <t>200MSP1T2B4M2QE</t>
+  </si>
+  <si>
+    <t>200MDP1T2B1M2QE</t>
+  </si>
+  <si>
+    <t>TAJS104K020RNJ</t>
+  </si>
+  <si>
+    <t>Polarized Cap Tantalium</t>
+  </si>
+  <si>
+    <t>FS57003PLT2B2M2QE</t>
+  </si>
+  <si>
+    <t>1x</t>
+  </si>
+  <si>
+    <t>2x</t>
+  </si>
+  <si>
+    <t>1N34A</t>
+  </si>
+  <si>
+    <t>1N4154</t>
+  </si>
+  <si>
+    <t>Diode Germanium</t>
+  </si>
+  <si>
+    <t>Diode Silicon</t>
+  </si>
+  <si>
+    <t>3x</t>
+  </si>
+  <si>
+    <t>10x</t>
+  </si>
+  <si>
+    <t>Ricordare di contare x2</t>
+  </si>
+  <si>
+    <t>Pot 100k lin</t>
+  </si>
+  <si>
+    <t>Pot 500k Log</t>
+  </si>
+  <si>
+    <t>PDB181-K420K-104B</t>
+  </si>
+  <si>
+    <t>PDB181-K420K-504A</t>
+  </si>
+  <si>
+    <t>Toggle2</t>
+  </si>
+  <si>
+    <t>Ferrite Bead</t>
+  </si>
+  <si>
+    <t>BLM21PG221SN1D</t>
+  </si>
+  <si>
+    <t>Schottky Diode</t>
+  </si>
+  <si>
+    <t>MP01EA03</t>
+  </si>
+  <si>
+    <t>Connettore jack alimentazione</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,6 +147,14 @@
       <color rgb="FF474747"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -85,9 +177,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -368,19 +461,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B6:D15"/>
+  <dimension ref="B6:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="3" max="3" width="23.7109375" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="25.20703125" customWidth="1"/>
+    <col min="3" max="3" width="23.68359375" customWidth="1"/>
+    <col min="4" max="4" width="17.41796875" customWidth="1"/>
+    <col min="5" max="5" width="20.1015625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="C6" t="s">
         <v>0</v>
       </c>
@@ -388,20 +483,155 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" t="s">
         <v>3</v>
       </c>
       <c r="C14" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" t="s">
         <v>4</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B30" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>